<commit_message>
adding pressure-depth to docs
</commit_message>
<xml_diff>
--- a/docs/Examples/Converting_Pressures_to_depths/Example_Pressure_data.xlsx
+++ b/docs/Examples/Converting_Pressures_to_depths/Example_Pressure_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\Box\Berkeley_new\DiadFit_outer\docs\Examples\Converting_Pressures_to_depths\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62969161-AF72-41FC-9620-849849EA8E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E50054C-3ABF-4B8A-93BC-7DA30ECA3658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{F7B1713C-5544-491F-BB52-1AFBE965CBC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Validate" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
   <si>
     <t>Fluid inclusion Name</t>
   </si>
@@ -282,6 +283,24 @@
   </si>
   <si>
     <t>P_kbar</t>
+  </si>
+  <si>
+    <t>four-step profile</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>Pressure (kbar)</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Fo</t>
   </si>
 </sst>
 </file>
@@ -656,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A0FF9C-F36F-4837-9A07-8D44EBEEB507}">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -668,183 +687,249 @@
     <col min="2" max="2" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0.73428628274174501</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>0.87470681125170602</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>0.75697837118984401</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>0.87470681125170602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>0.76630283390527298</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>0.87401540072509698</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>0.71000853150373699</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>0.87401540072509698</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>0.72671519734293</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>0.87357226608473104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>0.75912341069414502</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>0.87189156801720102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>0.86923334688528997</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>0.87189156801720102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>1.3148308338414401</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>0.87150404501761503</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <v>1.4877014917695299</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>0.87150404501761503</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
         <v>1.2434966545695201</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>0.87150404501761503</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
         <v>0.985225138455747</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>0.87130224255418198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13">
         <v>0.94678505773618005</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <v>0.87130224255418198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>1.22398571128904</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>0.87130224255418198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15">
         <v>1.0251260233023201</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>0.878341382604513</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16">
         <v>0.57676124021453001</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>0.87572184762136496</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
         <v>0.77454634879456496</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>0.87035933890384598</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
         <v>0.78129037242330301</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <v>0.87035933890384598</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
         <v>0.98079134081382402</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19">
+        <v>0.87035933890384598</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
         <v>0.83745093241267998</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <v>0.87035933890384598</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
         <v>0.92315245031121296</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>0.87035933890384598</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <v>1.0582801192636899</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <v>0.87035933890384598</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -852,71 +937,95 @@
         <v>0.67820873049771302</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24">
         <v>0.64646660727977701</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>0.86322923495974702</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25">
         <v>0.65732525483255799</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25">
+        <v>0.86941972359887398</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26">
         <v>0.93125902241564995</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <v>0.86941972359887398</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27">
         <v>0.98427230766271501</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27">
+        <v>0.86941972359887398</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28">
         <v>0.85736028115718199</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <v>0.87074063815980096</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29">
         <v>0.61482154144785595</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <v>0.86247734730096004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30">
         <v>0.73160923532615396</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30">
+        <v>0.86247734730096004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31">
         <v>0.15257503924618701</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>0.87546356242025702</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -924,103 +1033,139 @@
         <v>0.12692192237498501</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33">
         <v>0.70936072431271202</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>0.86890709350051698</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34">
         <v>0.15645752370247701</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <v>0.86489650332994295</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35">
         <v>1.11727734139713</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <v>0.87164796795223198</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36">
         <v>0.93667052519732996</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <v>0.873149079124657</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37">
         <v>0.183451446347972</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37">
+        <v>0.87364014130122003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38">
         <v>1.3481449034567901</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38">
+        <v>0.87364014130122003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39">
         <v>0.70193024173660701</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39">
+        <v>0.87450771124067395</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40">
         <v>0.68673376077596604</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40">
+        <v>0.87450771124067395</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
       <c r="B41">
         <v>0.75191639872869298</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41">
+        <v>0.87450771124067395</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
       <c r="B42">
         <v>0.72508009844264998</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42">
+        <v>0.84285782048410096</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43">
         <v>0.64683413797697098</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43">
+        <v>0.84285782048410096</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44">
         <v>0.71162881224494001</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44">
+        <v>0.84285782048410096</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1028,71 +1173,95 @@
         <v>0.26275612708817803</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
       <c r="B46">
         <v>0.67535567712917299</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46">
+        <v>0.87241983258838296</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47">
         <v>0.69190680781230096</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47">
+        <v>0.87241983258838296</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
       <c r="B48">
         <v>0.77663277597966796</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48">
+        <v>0.87259307613466897</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
       <c r="B49">
         <v>0.77003809119120703</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49">
+        <v>0.87259307613466897</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
       <c r="B50">
         <v>0.68140754609590104</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C50">
+        <v>0.872880597902708</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>50</v>
       </c>
       <c r="B51">
         <v>0.80414378401984399</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C51">
+        <v>0.87263396152918804</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
       <c r="B52">
         <v>0.86231971628073201</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C52">
+        <v>0.87263396152918804</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
       <c r="B53">
         <v>0.833433671621711</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C53">
+        <v>0.87263396152918804</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1100,7 +1269,7 @@
         <v>0.53994078936849499</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1108,7 +1277,7 @@
         <v>0.664428968810853</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1116,7 +1285,7 @@
         <v>0.397073849443495</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1124,7 +1293,7 @@
         <v>0.54889403753680099</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1132,39 +1301,51 @@
         <v>0.51980848620180697</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>58</v>
       </c>
       <c r="B59">
         <v>0.56518161716114801</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C59">
+        <v>0.84900082720034098</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>59</v>
       </c>
       <c r="B60">
         <v>7.8855460397450006E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C60">
+        <v>0.847291723223494</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>60</v>
       </c>
       <c r="B61">
         <v>0.59013110255352597</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C61">
+        <v>0.84980348227613201</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>61</v>
       </c>
       <c r="B62">
         <v>0.69804410780931303</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C62">
+        <v>0.84980348227613201</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1172,7 +1353,7 @@
         <v>0.63274137396699104</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1180,7 +1361,7 @@
         <v>0.74225604919464205</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -1188,7 +1369,7 @@
         <v>0.51715223636858898</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1196,7 +1377,7 @@
         <v>0.53578073714033103</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1204,7 +1385,7 @@
         <v>0.53316978508898605</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -1212,7 +1393,7 @@
         <v>0.64206582848031402</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -1220,7 +1401,7 @@
         <v>0.60023758898911805</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -1228,7 +1409,7 @@
         <v>0.620414458708203</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -1236,7 +1417,7 @@
         <v>0.53224784565461403</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -1244,7 +1425,7 @@
         <v>0.67683777782764598</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1252,39 +1433,51 @@
         <v>0.651554430971506</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>73</v>
       </c>
       <c r="B74">
         <v>0.51095270981366903</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C74">
+        <v>0.85195359495444101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>74</v>
       </c>
       <c r="B75">
         <v>0.53401687073313997</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C75">
+        <v>0.85265796427009199</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>75</v>
       </c>
       <c r="B76">
         <v>0.51527621999301099</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C76">
+        <v>0.85265796427009199</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>76</v>
       </c>
       <c r="B77">
         <v>0.55815294231857904</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C77">
+        <v>0.85319080909363398</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -1292,7 +1485,7 @@
         <v>0.64525965005674202</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -1300,7 +1493,7 @@
         <v>0.49639867500984503</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -1308,12 +1501,123 @@
         <v>0.663104460188774</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>80</v>
       </c>
       <c r="B81">
         <v>1.02309013862141</v>
+      </c>
+      <c r="C81">
+        <v>0.86624459823279298</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B6B7742-0D74-4FC5-8C43-36D7857C04BA}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1035</v>
+      </c>
+      <c r="D3">
+        <f>C3*9.8*B3/10^5</f>
+        <v>0.10143000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>2400</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D6" si="0">C4*9.8*B4/10^5</f>
+        <v>0.94079999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>2700</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>2.1168000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>3300</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2.2638000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <f>SUM(B2:B5)</f>
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7">
+        <f>SUM(D2:D5)</f>
+        <v>3.1590300000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B3:B6)</f>
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8">
+        <f>SUM(D3:D6)</f>
+        <v>5.4228300000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>